<commit_message>
update more precise measurement of Sekara S9
</commit_message>
<xml_diff>
--- a/Contact_data/Data/Sekara/Sekara_S9.xlsx
+++ b/Contact_data/Data/Sekara/Sekara_S9.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eva/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eva/Desktop/Contact_data/Data/Sekara/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16180" activeTab="1"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16180"/>
   </bookViews>
   <sheets>
-    <sheet name="FigureS9" sheetId="2" r:id="rId1"/>
-    <sheet name="FigureS15" sheetId="3" r:id="rId2"/>
+    <sheet name="FigureS9" sheetId="3" r:id="rId1"/>
+    <sheet name="FigureS9old" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Sekara_S19" localSheetId="0">FigureS9!$A$1:$B$144</definedName>
+    <definedName name="Sekara_S19" localSheetId="0">FigureS9!$A$1:$B$143</definedName>
+    <definedName name="Sekara_S19" localSheetId="1">FigureS9old!$A$1:$B$144</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,15 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="Sekara-S19" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/eva/Downloads/Sekara-S19.csv" decimal="," thousands=" " tab="0" semicolon="1">
+    <textPr sourceFile="/Users/eva/Downloads/Sekara-S19.csv" decimal="," thousands=" " tab="0" semicolon="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="Sekara-S191" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr sourceFile="/Users/eva/Downloads/Sekara-S19.csv" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -91,6 +100,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Sekara-S19" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Sekara-S19" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -391,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B144"/>
+  <dimension ref="A1:B143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -551,7 +564,7 @@
         <v>20.9678919666074</v>
       </c>
       <c r="B19">
-        <v>5.5072227473618703E-3</v>
+        <v>5.6402108125492099E-3</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -559,7 +572,7 @@
         <v>21.838490433297999</v>
       </c>
       <c r="B20">
-        <v>4.0384770256365003E-3</v>
+        <v>3.9905822769950002E-3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -567,15 +580,15 @@
         <v>22.931054592658501</v>
       </c>
       <c r="B21">
-        <v>4.1359979124029299E-3</v>
+        <v>3.9905822769950097E-3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>23.883164656930202</v>
+        <v>23.980523369427601</v>
       </c>
       <c r="B22">
-        <v>4.0384770256365003E-3</v>
+        <v>3.9905822769950002E-3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -588,7 +601,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>26.119275770101702</v>
+        <v>25.907622590372899</v>
       </c>
       <c r="B24">
         <v>4.1359979124029299E-3</v>
@@ -596,10 +609,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>26.983321403524901</v>
+        <v>26.764666574617301</v>
       </c>
       <c r="B25">
-        <v>3.3366915550634701E-3</v>
+        <v>3.2971197059952499E-3</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -612,10 +625,10 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>28.798108100118402</v>
+        <v>28.915502372077899</v>
       </c>
       <c r="B27">
-        <v>2.5664122812420198E-3</v>
+        <v>2.5359756413056598E-3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -636,7 +649,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>32.536249606832001</v>
+        <v>31.881119921154902</v>
       </c>
       <c r="B30">
         <v>2.0704377436825999E-3</v>
@@ -647,15 +660,15 @@
         <v>32.8020555742347</v>
       </c>
       <c r="B31">
-        <v>1.7942626234056401E-3</v>
+        <v>1.88196437870106E-3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>34.164015056509299</v>
+        <v>33.887172678387401</v>
       </c>
       <c r="B32">
-        <v>1.8819643787010699E-3</v>
+        <v>1.90455161149408E-3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -748,10 +761,10 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>45.419653450654103</v>
+        <v>45.977374711490597</v>
       </c>
       <c r="B44">
-        <v>1.19596978358375E-3</v>
+        <v>1.16777053486286E-3</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -948,10 +961,10 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>69.907370715725506</v>
+        <v>70.192345161312005</v>
       </c>
       <c r="B69">
-        <v>3.2193783617504902E-4</v>
+        <v>3.0329502389060101E-4</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -959,7 +972,7 @@
         <v>68.778995756320597</v>
       </c>
       <c r="B70">
-        <v>2.2507725307074501E-4</v>
+        <v>2.1716386615316401E-4</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -983,7 +996,7 @@
         <v>92.938975302017099</v>
       </c>
       <c r="B73">
-        <v>1.30013855507606E-4</v>
+        <v>1.3001385550760701E-4</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -991,7 +1004,7 @@
         <v>89.962932635377996</v>
       </c>
       <c r="B74">
-        <v>8.6661027547453104E-5</v>
+        <v>8.7701128425795205E-5</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -999,15 +1012,15 @@
         <v>83.610627742964297</v>
       </c>
       <c r="B75">
-        <v>8.6661027547453104E-5</v>
+        <v>8.8753712537578699E-5</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>104.15205528565799</v>
+        <v>105.002928946474</v>
       </c>
       <c r="B76">
-        <v>8.8753712537578903E-5</v>
+        <v>8.7701128425795395E-5</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1052,7 +1065,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>162.93490595486301</v>
+        <v>160.95844988807801</v>
       </c>
       <c r="B82">
         <v>8.8753712537578903E-5</v>
@@ -1060,7 +1073,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>181.11337767883001</v>
+        <v>178.19002641996099</v>
       </c>
       <c r="B83">
         <v>1.30013855507606E-4</v>
@@ -1100,7 +1113,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>92.185859870465606</v>
+        <v>91.438847183767805</v>
       </c>
       <c r="B88">
         <v>2.1977025491085999E-4</v>
@@ -1140,7 +1153,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>76.452594131278104</v>
+        <v>77.391377982622103</v>
       </c>
       <c r="B93">
         <v>3.0693515405837E-4</v>
@@ -1148,7 +1161,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>77.7068606678951</v>
+        <v>80.277463093402204</v>
       </c>
       <c r="B94">
         <v>3.0693515405837E-4</v>
@@ -1156,79 +1169,79 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>80.277463093402204</v>
+        <v>88.151494977620899</v>
       </c>
       <c r="B95">
-        <v>3.0693515405837E-4</v>
+        <v>3.0693515405837097E-4</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>89.233933067487698</v>
+        <v>80.933292483575599</v>
       </c>
       <c r="B96">
-        <v>3.1434700466778301E-4</v>
+        <v>2.59721422005409E-4</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>80.933292483575599</v>
+        <v>87.0821872315381</v>
       </c>
       <c r="B97">
-        <v>2.59721422005409E-4</v>
+        <v>2.6283858420388697E-4</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>87.0821872315381</v>
+        <v>94.080200268486905</v>
       </c>
       <c r="B98">
-        <v>2.5972142200540998E-4</v>
+        <v>2.6283858420388697E-4</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>94.463714233290503</v>
+        <v>84.293687531997193</v>
       </c>
       <c r="B99">
-        <v>2.5972142200540998E-4</v>
+        <v>3.0693515405837E-4</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>84.293687531997193</v>
+        <v>108.918706100471</v>
       </c>
       <c r="B100">
-        <v>3.0693515405837E-4</v>
+        <v>2.62838584203888E-4</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>109.362708607892</v>
+        <v>117.671523978507</v>
       </c>
       <c r="B101">
-        <v>2.7241634430974103E-4</v>
+        <v>2.62838584203888E-4</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>117.671523978507</v>
+        <v>127.645958006849</v>
       </c>
       <c r="B102">
-        <v>2.7241634430974103E-4</v>
+        <v>2.6283858420388697E-4</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>128.688765883081</v>
+        <v>124.56796234785099</v>
       </c>
       <c r="B103">
-        <v>2.65993158411342E-4</v>
+        <v>2.1977025491085999E-4</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>125.585624436733</v>
+        <v>113.903508731185</v>
       </c>
       <c r="B104">
         <v>2.1977025491085999E-4</v>
@@ -1236,103 +1249,103 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>113.903508731185</v>
+        <v>107.59748498951799</v>
       </c>
       <c r="B105">
-        <v>2.1977025491085999E-4</v>
+        <v>2.1977025491085899E-4</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>107.59748498951799</v>
+        <v>103.308076537145</v>
       </c>
       <c r="B106">
-        <v>2.14588388140686E-4</v>
+        <v>2.1977025491085999E-4</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>102.470936829168</v>
+        <v>143.62955543959299</v>
       </c>
       <c r="B107">
-        <v>2.1977025491085999E-4</v>
+        <v>1.75195648935232E-4</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>143.04643269540799</v>
+        <v>113.44107099418601</v>
       </c>
       <c r="B108">
-        <v>1.7729833746196901E-4</v>
+        <v>1.75195648935232E-4</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>112.980510711737</v>
+        <v>117.193788447232</v>
       </c>
       <c r="B109">
-        <v>1.7311789746714799E-4</v>
+        <v>1.75195648935232E-4</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>116.717992478139</v>
+        <v>122.05973933491801</v>
       </c>
       <c r="B110">
-        <v>1.7311789746714799E-4</v>
+        <v>1.75195648935232E-4</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>121.56418805414199</v>
+        <v>127.127727193635</v>
       </c>
       <c r="B111">
-        <v>1.7311789746714799E-4</v>
+        <v>1.75195648935232E-4</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>127.645958006849</v>
+        <v>132.94588875320201</v>
       </c>
       <c r="B112">
-        <v>1.7311789746714799E-4</v>
+        <v>1.75195648935232E-4</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>132.94588875320201</v>
+        <v>130.80000899418499</v>
       </c>
       <c r="B113">
-        <v>1.7311789746714799E-4</v>
+        <v>1.30013855507606E-4</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>130.80000899418499</v>
+        <v>138.465875554245</v>
       </c>
       <c r="B114">
-        <v>1.30013855507606E-4</v>
+        <v>1.3157427463875599E-4</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>138.465875554245</v>
+        <v>143.04643269540799</v>
       </c>
       <c r="B115">
-        <v>1.3315342183435201E-4</v>
+        <v>1.3157427463875599E-4</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>144.21505525902799</v>
+        <v>121.070648665847</v>
       </c>
       <c r="B116">
-        <v>1.3315342183435201E-4</v>
+        <v>1.3157427463875599E-4</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>121.070648665847</v>
+        <v>114.83404721348499</v>
       </c>
       <c r="B117">
         <v>1.3157427463875599E-4</v>
@@ -1340,47 +1353,47 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>114.83404721348499</v>
+        <v>111.15689214501499</v>
       </c>
       <c r="B118">
-        <v>1.3315342183435201E-4</v>
+        <v>1.3157427463875599E-4</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>111.15689214501499</v>
+        <v>105.43096895363099</v>
       </c>
       <c r="B119">
-        <v>1.3315342183435201E-4</v>
+        <v>1.3157427463875599E-4</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>105.43096895363099</v>
+        <v>98.786965840619999</v>
       </c>
       <c r="B120">
-        <v>1.3157427463875599E-4</v>
+        <v>4.3902277105074097E-5</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>98.385899873142904</v>
+        <v>112.064992052261</v>
       </c>
       <c r="B121">
-        <v>4.4429189816248803E-5</v>
+        <v>4.3902277105074097E-5</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>112.064992052261</v>
+        <v>122.557310709571</v>
       </c>
       <c r="B122">
-        <v>4.3381613371347498E-5</v>
+        <v>4.4429189816248803E-5</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>122.557310709571</v>
+        <v>129.740093012752</v>
       </c>
       <c r="B123">
         <v>4.4429189816248803E-5</v>
@@ -1388,7 +1401,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>129.740093012752</v>
+        <v>134.03199458897799</v>
       </c>
       <c r="B124">
         <v>4.4429189816248803E-5</v>
@@ -1396,7 +1409,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
-        <v>134.03199458897799</v>
+        <v>139.59707710478301</v>
       </c>
       <c r="B125">
         <v>4.4429189816248803E-5</v>
@@ -1404,7 +1417,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>139.59707710478301</v>
+        <v>148.98579966508399</v>
       </c>
       <c r="B126">
         <v>4.4429189816248803E-5</v>
@@ -1412,7 +1425,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>148.98579966508399</v>
+        <v>314.94391046118398</v>
       </c>
       <c r="B127">
         <v>4.4429189816248803E-5</v>
@@ -1420,7 +1433,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>314.94391046118398</v>
+        <v>296.29986169528598</v>
       </c>
       <c r="B128">
         <v>4.4429189816248803E-5</v>
@@ -1428,7 +1441,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
-        <v>296.29986169528598</v>
+        <v>281.03683826106101</v>
       </c>
       <c r="B129">
         <v>4.4429189816248803E-5</v>
@@ -1436,7 +1449,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>281.03683826106101</v>
+        <v>272.03762540290001</v>
       </c>
       <c r="B130">
         <v>4.4429189816248803E-5</v>
@@ -1444,7 +1457,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
-        <v>272.03762540290001</v>
+        <v>261.19275770101802</v>
       </c>
       <c r="B131">
         <v>4.4429189816248803E-5</v>
@@ -1452,7 +1465,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>261.19275770101802</v>
+        <v>252.82898148539499</v>
       </c>
       <c r="B132">
         <v>4.4429189816248803E-5</v>
@@ -1460,7 +1473,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
-        <v>252.82898148539499</v>
+        <v>238.83164656930199</v>
       </c>
       <c r="B133">
         <v>4.4429189816248803E-5</v>
@@ -1468,7 +1481,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>238.83164656930199</v>
+        <v>231.183906016707</v>
       </c>
       <c r="B134">
         <v>4.4429189816248803E-5</v>
@@ -1476,7 +1489,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135">
-        <v>231.183906016707</v>
+        <v>220.16900703270201</v>
       </c>
       <c r="B135">
         <v>4.4429189816248803E-5</v>
@@ -1484,7 +1497,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
-        <v>220.16900703270201</v>
+        <v>207.979821633645</v>
       </c>
       <c r="B136">
         <v>4.4429189816248803E-5</v>
@@ -1492,7 +1505,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137">
-        <v>207.979821633645</v>
+        <v>198.07049548081099</v>
       </c>
       <c r="B137">
         <v>4.4429189816248803E-5</v>
@@ -1500,7 +1513,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>198.07049548081099</v>
+        <v>190.17435127666201</v>
       </c>
       <c r="B138">
         <v>4.4429189816248803E-5</v>
@@ -1508,15 +1521,15 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
-        <v>190.17435127666201</v>
+        <v>156.43945336266401</v>
       </c>
       <c r="B139">
-        <v>4.4429189816248803E-5</v>
+        <v>4.4429189816248702E-5</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>156.43945336266401</v>
+        <v>162.93490595486301</v>
       </c>
       <c r="B140">
         <v>4.4429189816248702E-5</v>
@@ -1524,15 +1537,15 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>162.93490595486301</v>
+        <v>182.592989408677</v>
       </c>
       <c r="B141">
-        <v>4.4429189816248702E-5</v>
+        <v>4.4429189816248803E-5</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>182.592989408677</v>
+        <v>175.31386097747</v>
       </c>
       <c r="B142">
         <v>4.4429189816248803E-5</v>
@@ -1540,17 +1553,9 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>175.31386097747</v>
+        <v>168.32491734957699</v>
       </c>
       <c r="B143">
-        <v>4.4429189816248803E-5</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A144">
-        <v>168.32491734957699</v>
-      </c>
-      <c r="B144">
         <v>4.4429189816248803E-5</v>
       </c>
     </row>
@@ -1561,14 +1566,1170 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>2.9993821469659001</v>
+      </c>
+      <c r="B1">
+        <v>0.28234311515510602</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3.9875552523887001</v>
+      </c>
+      <c r="B2">
+        <v>0.16703132547319699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>4.9672163253953396</v>
+      </c>
+      <c r="B3">
+        <v>0.12544275856537199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>5.9894253860490796</v>
+      </c>
+      <c r="B4">
+        <v>7.9717634675489604E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>6.9907370715725499</v>
+      </c>
+      <c r="B5">
+        <v>6.0587553983754303E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>7.9626948106928701</v>
+      </c>
+      <c r="B6">
+        <v>4.0869466044126099E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>8.9597691428631201</v>
+      </c>
+      <c r="B7">
+        <v>3.1434700466778299E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>2.53597564130566E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>10.9808521072791</v>
+      </c>
+      <c r="B9">
+        <v>2.09528702341884E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>11.960202034054699</v>
+      </c>
+      <c r="B10">
+        <v>1.5002574881357599E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>12.974009301275199</v>
+      </c>
+      <c r="B11">
+        <v>1.33153421834352E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>13.9597077104783</v>
+      </c>
+      <c r="B12">
+        <v>1.10014714790277E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>14.959313398799001</v>
+      </c>
+      <c r="B13">
+        <v>1.04887899583449E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>15.9005968908527</v>
+      </c>
+      <c r="B14">
+        <v>8.4617685061913108E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>16.970005332974502</v>
+      </c>
+      <c r="B15">
+        <v>8.0674401335104305E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>17.964575573499999</v>
+      </c>
+      <c r="B16">
+        <v>6.3549012782548398E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>18.863330524977801</v>
+      </c>
+      <c r="B17">
+        <v>6.9913265164757502E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>19.968863894545098</v>
+      </c>
+      <c r="B18">
+        <v>6.0587553983754401E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>20.9678919666074</v>
+      </c>
+      <c r="B19">
+        <v>5.5072227473618703E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>21.838490433297999</v>
+      </c>
+      <c r="B20">
+        <v>4.0384770256365003E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>22.931054592658501</v>
+      </c>
+      <c r="B21">
+        <v>4.1359979124029299E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>23.883164656930202</v>
+      </c>
+      <c r="B22">
+        <v>4.0384770256365003E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>24.8748068574508</v>
+      </c>
+      <c r="B23">
+        <v>4.2358737273502801E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>26.119275770101702</v>
+      </c>
+      <c r="B24">
+        <v>4.1359979124029299E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>26.983321403524901</v>
+      </c>
+      <c r="B25">
+        <v>3.3366915550634701E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>27.875950327817499</v>
+      </c>
+      <c r="B26">
+        <v>2.3327900146215999E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>28.798108100118402</v>
+      </c>
+      <c r="B27">
+        <v>2.5664122812420198E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>29.993821469659</v>
+      </c>
+      <c r="B28">
+        <v>2.38912207975942E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>30.986040040290199</v>
+      </c>
+      <c r="B29">
+        <v>2.2240792540283699E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>32.536249606832001</v>
+      </c>
+      <c r="B30">
+        <v>2.0704377436825999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>32.8020555742347</v>
+      </c>
+      <c r="B31">
+        <v>1.7942626234056401E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>34.164015056509299</v>
+      </c>
+      <c r="B32">
+        <v>1.8819643787010699E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>35.873216455049203</v>
+      </c>
+      <c r="B33">
+        <v>2.0704377436825999E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>37.0599299117182</v>
+      </c>
+      <c r="B34">
+        <v>2.0704377436825999E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>37.975657368770896</v>
+      </c>
+      <c r="B35">
+        <v>1.75195648935232E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35.0081862868632</v>
+      </c>
+      <c r="B36">
+        <v>1.48246502458189E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>42.905091641376799</v>
+      </c>
+      <c r="B37">
+        <v>1.55492642634321E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>43.965249352332002</v>
+      </c>
+      <c r="B38">
+        <v>1.4475106298120299E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>40.529743159641598</v>
+      </c>
+      <c r="B39">
+        <v>1.3475152186759199E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>38.598678690478998</v>
+      </c>
+      <c r="B40">
+        <v>1.2248499859720599E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>39.875552523887002</v>
+      </c>
+      <c r="B41">
+        <v>1.14023618390054E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41.870498083671002</v>
+      </c>
+      <c r="B42">
+        <v>1.0614675837582199E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>44.6865347666891</v>
+      </c>
+      <c r="B43">
+        <v>1.11335105336319E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>45.419653450654103</v>
+      </c>
+      <c r="B44">
+        <v>1.19596978358375E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>46.922170349708097</v>
+      </c>
+      <c r="B45">
+        <v>1.25442758565372E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>47.691966440525199</v>
+      </c>
+      <c r="B46">
+        <v>1.0120019449085401E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>50.899531029640102</v>
+      </c>
+      <c r="B47">
+        <v>9.6484146305493503E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>49.6721632539534</v>
+      </c>
+      <c r="B48">
+        <v>8.7701128425795205E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>51.734578933839998</v>
+      </c>
+      <c r="B49">
+        <v>7.9717634675489804E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>56.1198637258844</v>
+      </c>
+      <c r="B50">
+        <v>6.1314722468810805E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>58.9275006329486</v>
+      </c>
+      <c r="B51">
+        <v>7.0752360321641404E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>53.445998401141502</v>
+      </c>
+      <c r="B52">
+        <v>6.9084121346304095E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>59.894253860490799</v>
+      </c>
+      <c r="B53">
+        <v>9.6484146305493503E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>64.971194003777697</v>
+      </c>
+      <c r="B54">
+        <v>7.4210664647083398E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>61.875601619548199</v>
+      </c>
+      <c r="B55">
+        <v>6.1314722468810805E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>63.4045086482352</v>
+      </c>
+      <c r="B56">
+        <v>5.1883098755244397E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>60.876867455313601</v>
+      </c>
+      <c r="B57">
+        <v>4.8298964943584502E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>54.766615259352101</v>
+      </c>
+      <c r="B58">
+        <v>4.3902277105073998E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>57.976351770478502</v>
+      </c>
+      <c r="B59">
+        <v>3.5417899226997102E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>56.808976010485601</v>
+      </c>
+      <c r="B60">
+        <v>3.0329502389059998E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>66.847987828123195</v>
+      </c>
+      <c r="B61">
+        <v>5.7079043119940198E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>72.809963396592593</v>
+      </c>
+      <c r="B62">
+        <v>6.1314722468810805E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>77.077176127945606</v>
+      </c>
+      <c r="B63">
+        <v>5.1883098755244397E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>74.609051597462994</v>
+      </c>
+      <c r="B64">
+        <v>4.3902277105073998E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>70.478481293195699</v>
+      </c>
+      <c r="B65">
+        <v>4.8878646459976898E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>63.922493878942298</v>
+      </c>
+      <c r="B66">
+        <v>3.9905822769949998E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66.037098900909896</v>
+      </c>
+      <c r="B67">
+        <v>3.5417899226997102E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67.668833898566902</v>
+      </c>
+      <c r="B68">
+        <v>3.0693515405837E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>69.907370715725506</v>
+      </c>
+      <c r="B69">
+        <v>3.2193783617504902E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>68.778995756320597</v>
+      </c>
+      <c r="B70">
+        <v>2.2507725307074501E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>82.933103014610893</v>
+      </c>
+      <c r="B71">
+        <v>1.7729833746196901E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>85.676593536964006</v>
+      </c>
+      <c r="B72">
+        <v>3.6273168408446999E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>92.938975302017099</v>
+      </c>
+      <c r="B73">
+        <v>1.30013855507606E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>89.962932635377996</v>
+      </c>
+      <c r="B74">
+        <v>8.6661027547453104E-5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>83.610627742964297</v>
+      </c>
+      <c r="B75">
+        <v>8.6661027547453104E-5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>104.15205528565799</v>
+      </c>
+      <c r="B76">
+        <v>8.8753712537578903E-5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>128.688765883081</v>
+      </c>
+      <c r="B77">
+        <v>8.7701128425795205E-5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>136.786237184687</v>
+      </c>
+      <c r="B78">
+        <v>8.7701128425795205E-5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>146.58101968369101</v>
+      </c>
+      <c r="B79">
+        <v>8.8753712537578903E-5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>151.430032003756</v>
+      </c>
+      <c r="B80">
+        <v>8.8753712537578903E-5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>156.43945336266401</v>
+      </c>
+      <c r="B81">
+        <v>8.8753712537578903E-5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>162.93490595486301</v>
+      </c>
+      <c r="B82">
+        <v>8.8753712537578903E-5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>181.11337767883001</v>
+      </c>
+      <c r="B83">
+        <v>1.30013855507606E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>173.893234446588</v>
+      </c>
+      <c r="B84">
+        <v>1.30013855507606E-4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>153.914363947483</v>
+      </c>
+      <c r="B85">
+        <v>1.30013855507606E-4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>107.59748498951799</v>
+      </c>
+      <c r="B86">
+        <v>3.5417899226997102E-4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>96.013467737846796</v>
+      </c>
+      <c r="B87">
+        <v>3.1434700466778301E-4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>92.185859870465606</v>
+      </c>
+      <c r="B88">
+        <v>2.1977025491085999E-4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>96.797852938481299</v>
+      </c>
+      <c r="B89">
+        <v>1.75195648935232E-4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>101.64058074270601</v>
+      </c>
+      <c r="B90">
+        <v>1.7729833746196901E-4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>100.816953307817</v>
+      </c>
+      <c r="B91">
+        <v>2.65993158411342E-4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>74.004469634848505</v>
+      </c>
+      <c r="B92">
+        <v>3.0693515405837E-4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>76.452594131278104</v>
+      </c>
+      <c r="B93">
+        <v>3.0693515405837E-4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>77.7068606678951</v>
+      </c>
+      <c r="B94">
+        <v>3.0693515405837E-4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>80.277463093402204</v>
+      </c>
+      <c r="B95">
+        <v>3.0693515405837E-4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>89.233933067487698</v>
+      </c>
+      <c r="B96">
+        <v>3.1434700466778301E-4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>80.933292483575599</v>
+      </c>
+      <c r="B97">
+        <v>2.59721422005409E-4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>87.0821872315381</v>
+      </c>
+      <c r="B98">
+        <v>2.5972142200540998E-4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>94.463714233290503</v>
+      </c>
+      <c r="B99">
+        <v>2.5972142200540998E-4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>84.293687531997193</v>
+      </c>
+      <c r="B100">
+        <v>3.0693515405837E-4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>109.362708607892</v>
+      </c>
+      <c r="B101">
+        <v>2.7241634430974103E-4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>117.671523978507</v>
+      </c>
+      <c r="B102">
+        <v>2.7241634430974103E-4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>128.688765883081</v>
+      </c>
+      <c r="B103">
+        <v>2.65993158411342E-4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>125.585624436733</v>
+      </c>
+      <c r="B104">
+        <v>2.1977025491085999E-4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>113.903508731185</v>
+      </c>
+      <c r="B105">
+        <v>2.1977025491085999E-4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>107.59748498951799</v>
+      </c>
+      <c r="B106">
+        <v>2.14588388140686E-4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>102.470936829168</v>
+      </c>
+      <c r="B107">
+        <v>2.1977025491085999E-4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>143.04643269540799</v>
+      </c>
+      <c r="B108">
+        <v>1.7729833746196901E-4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>112.980510711737</v>
+      </c>
+      <c r="B109">
+        <v>1.7311789746714799E-4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>116.717992478139</v>
+      </c>
+      <c r="B110">
+        <v>1.7311789746714799E-4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>121.56418805414199</v>
+      </c>
+      <c r="B111">
+        <v>1.7311789746714799E-4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>127.645958006849</v>
+      </c>
+      <c r="B112">
+        <v>1.7311789746714799E-4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>132.94588875320201</v>
+      </c>
+      <c r="B113">
+        <v>1.7311789746714799E-4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>130.80000899418499</v>
+      </c>
+      <c r="B114">
+        <v>1.30013855507606E-4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>138.465875554245</v>
+      </c>
+      <c r="B115">
+        <v>1.3315342183435201E-4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>144.21505525902799</v>
+      </c>
+      <c r="B116">
+        <v>1.3315342183435201E-4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>121.070648665847</v>
+      </c>
+      <c r="B117">
+        <v>1.3157427463875599E-4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>114.83404721348499</v>
+      </c>
+      <c r="B118">
+        <v>1.3315342183435201E-4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>111.15689214501499</v>
+      </c>
+      <c r="B119">
+        <v>1.3315342183435201E-4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>105.43096895363099</v>
+      </c>
+      <c r="B120">
+        <v>1.3157427463875599E-4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>98.385899873142904</v>
+      </c>
+      <c r="B121">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>112.064992052261</v>
+      </c>
+      <c r="B122">
+        <v>4.3381613371347498E-5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>122.557310709571</v>
+      </c>
+      <c r="B123">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>129.740093012752</v>
+      </c>
+      <c r="B124">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>134.03199458897799</v>
+      </c>
+      <c r="B125">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>139.59707710478301</v>
+      </c>
+      <c r="B126">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>148.98579966508399</v>
+      </c>
+      <c r="B127">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>314.94391046118398</v>
+      </c>
+      <c r="B128">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>296.29986169528598</v>
+      </c>
+      <c r="B129">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>281.03683826106101</v>
+      </c>
+      <c r="B130">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>272.03762540290001</v>
+      </c>
+      <c r="B131">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>261.19275770101802</v>
+      </c>
+      <c r="B132">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>252.82898148539499</v>
+      </c>
+      <c r="B133">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>238.83164656930199</v>
+      </c>
+      <c r="B134">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>231.183906016707</v>
+      </c>
+      <c r="B135">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>220.16900703270201</v>
+      </c>
+      <c r="B136">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>207.979821633645</v>
+      </c>
+      <c r="B137">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>198.07049548081099</v>
+      </c>
+      <c r="B138">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>190.17435127666201</v>
+      </c>
+      <c r="B139">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>156.43945336266401</v>
+      </c>
+      <c r="B140">
+        <v>4.4429189816248702E-5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>162.93490595486301</v>
+      </c>
+      <c r="B141">
+        <v>4.4429189816248702E-5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>182.592989408677</v>
+      </c>
+      <c r="B142">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>175.31386097747</v>
+      </c>
+      <c r="B143">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>168.32491734957699</v>
+      </c>
+      <c r="B144">
+        <v>4.4429189816248803E-5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>